<commit_message>
Added data from 1942
</commit_message>
<xml_diff>
--- a/catch_reconstruction_data/recreational/pre_1970/1938_1942_sportcatch.xlsx
+++ b/catch_reconstruction_data/recreational/pre_1970/1938_1942_sportcatch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markusmin/Documents/ESA_RF_2021/catch_reconstruction_data/recreational/pre_1970/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395B856E-E28A-044D-8993-B21D50F2F92A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F03201-2321-514B-8A18-71544AE27A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21800" yWindow="460" windowWidth="16560" windowHeight="19080" activeTab="4" xr2:uid="{4C5FAADC-2B74-A74C-8EAD-9330A1A21B32}"/>
+    <workbookView xWindow="21640" yWindow="460" windowWidth="16560" windowHeight="19080" activeTab="2" xr2:uid="{4C5FAADC-2B74-A74C-8EAD-9330A1A21B32}"/>
   </bookViews>
   <sheets>
     <sheet name="1938" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="1941" sheetId="5" r:id="rId4"/>
     <sheet name="1942" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="17">
   <si>
     <t>rock_cod</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>red_snapper</t>
+  </si>
+  <si>
+    <t>fisherman_days</t>
   </si>
 </sst>
 </file>
@@ -436,19 +439,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF166D5F-3F5C-5D4C-8933-E9CC9A3F753A}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -456,16 +461,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -473,16 +481,19 @@
         <v>41</v>
       </c>
       <c r="C2">
+        <v>6250</v>
+      </c>
+      <c r="D2">
         <v>261</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -490,16 +501,19 @@
         <v>38</v>
       </c>
       <c r="C3">
+        <v>7323</v>
+      </c>
+      <c r="D3">
         <v>240</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -507,16 +521,19 @@
         <v>42</v>
       </c>
       <c r="C4">
+        <v>11119</v>
+      </c>
+      <c r="D4">
         <v>410</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -524,16 +541,19 @@
         <v>47</v>
       </c>
       <c r="C5">
+        <v>11407</v>
+      </c>
+      <c r="D5">
         <v>401</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -541,16 +561,19 @@
         <v>45</v>
       </c>
       <c r="C6">
+        <v>12658</v>
+      </c>
+      <c r="D6">
         <v>699</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -558,16 +581,19 @@
         <v>50</v>
       </c>
       <c r="C7">
+        <v>26802</v>
+      </c>
+      <c r="D7">
         <v>906</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -575,16 +601,19 @@
         <v>37</v>
       </c>
       <c r="C8">
+        <v>22214</v>
+      </c>
+      <c r="D8">
         <v>314</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -592,16 +621,19 @@
         <v>23</v>
       </c>
       <c r="C9">
+        <v>18822</v>
+      </c>
+      <c r="D9">
         <v>266</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -609,16 +641,19 @@
         <v>16</v>
       </c>
       <c r="C10">
+        <v>6106</v>
+      </c>
+      <c r="D10">
         <v>308</v>
       </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -626,12 +661,15 @@
         <v>10</v>
       </c>
       <c r="C11">
+        <v>950</v>
+      </c>
+      <c r="D11">
         <v>206</v>
       </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11">
         <v>101</v>
       </c>
     </row>
@@ -642,7 +680,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052F72E4-C784-AA45-A54E-E0617FC0D279}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
@@ -650,11 +688,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -662,16 +702,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -679,16 +722,19 @@
         <v>67</v>
       </c>
       <c r="C2">
+        <v>11398</v>
+      </c>
+      <c r="D2">
         <v>564</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -696,16 +742,19 @@
         <v>67</v>
       </c>
       <c r="C3">
+        <v>17300</v>
+      </c>
+      <c r="D3">
         <v>1007</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -713,16 +762,19 @@
         <v>65</v>
       </c>
       <c r="C4">
+        <v>28016</v>
+      </c>
+      <c r="D4">
         <v>1772</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -730,16 +782,19 @@
         <v>69</v>
       </c>
       <c r="C5">
+        <v>41022</v>
+      </c>
+      <c r="D5">
         <v>1364</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -747,16 +802,19 @@
         <v>60</v>
       </c>
       <c r="C6">
+        <v>17722</v>
+      </c>
+      <c r="D6">
         <v>809</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -764,16 +822,19 @@
         <v>55</v>
       </c>
       <c r="C7">
+        <v>6597</v>
+      </c>
+      <c r="D7">
         <v>553</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -781,12 +842,15 @@
         <v>46</v>
       </c>
       <c r="C8">
+        <v>2908</v>
+      </c>
+      <c r="D8">
         <v>122</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8">
         <v>101</v>
       </c>
     </row>
@@ -797,19 +861,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6B639E-F9A6-9948-AEAF-EE211E08CDEE}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -817,16 +883,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -834,16 +903,19 @@
         <v>71</v>
       </c>
       <c r="C2">
+        <v>14314</v>
+      </c>
+      <c r="D2">
         <v>516</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -851,16 +923,19 @@
         <v>75</v>
       </c>
       <c r="C3">
+        <v>12481</v>
+      </c>
+      <c r="D3">
         <v>1175</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>17</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -868,16 +943,19 @@
         <v>76</v>
       </c>
       <c r="C4">
+        <v>17497</v>
+      </c>
+      <c r="D4">
         <v>1542</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>6</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -885,16 +963,19 @@
         <v>75</v>
       </c>
       <c r="C5">
+        <v>28944</v>
+      </c>
+      <c r="D5">
         <v>1884</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>23</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -902,16 +983,19 @@
         <v>74</v>
       </c>
       <c r="C6">
+        <v>35597</v>
+      </c>
+      <c r="D6">
         <v>1778</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -919,16 +1003,19 @@
         <v>67</v>
       </c>
       <c r="C7">
+        <v>29960</v>
+      </c>
+      <c r="D7">
         <v>762</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -936,16 +1023,19 @@
         <v>61</v>
       </c>
       <c r="C8">
+        <v>11522</v>
+      </c>
+      <c r="D8">
         <v>306</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -953,12 +1043,15 @@
         <v>50</v>
       </c>
       <c r="C9">
+        <v>3171</v>
+      </c>
+      <c r="D9">
         <v>111</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
       <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>130</v>
       </c>
     </row>
@@ -969,20 +1062,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF77C11-07D1-BB4E-BF6E-59F0A267CD60}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -990,16 +1083,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1007,16 +1103,19 @@
         <v>58</v>
       </c>
       <c r="C2">
+        <v>15438</v>
+      </c>
+      <c r="D2">
         <v>578</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1024,16 +1123,19 @@
         <v>54</v>
       </c>
       <c r="C3">
+        <v>13319</v>
+      </c>
+      <c r="D3">
         <v>474</v>
       </c>
-      <c r="D3">
-        <v>14</v>
-      </c>
       <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1041,16 +1143,19 @@
         <v>57</v>
       </c>
       <c r="C4">
+        <v>17878</v>
+      </c>
+      <c r="D4">
         <v>760</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>13</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1058,16 +1163,19 @@
         <v>49</v>
       </c>
       <c r="C5">
+        <v>20094</v>
+      </c>
+      <c r="D5">
         <v>882</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1075,16 +1183,19 @@
         <v>43</v>
       </c>
       <c r="C6">
+        <v>34216</v>
+      </c>
+      <c r="D6">
         <v>870</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1092,16 +1203,19 @@
         <v>34</v>
       </c>
       <c r="C7">
+        <v>20101</v>
+      </c>
+      <c r="D7">
         <v>221</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>11</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1109,16 +1223,19 @@
         <v>26</v>
       </c>
       <c r="C8">
+        <v>5824</v>
+      </c>
+      <c r="D8">
         <v>154</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1126,12 +1243,15 @@
         <v>18</v>
       </c>
       <c r="C9">
+        <v>1538</v>
+      </c>
+      <c r="D9">
         <v>167</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
       <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>128</v>
       </c>
     </row>
@@ -1142,20 +1262,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0AFF23-2D8C-B045-89E3-0FEE5A4496B6}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1163,16 +1283,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1180,16 +1303,19 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1197,16 +1323,19 @@
         <v>8</v>
       </c>
       <c r="C3">
+        <v>1157</v>
+      </c>
+      <c r="D3">
         <v>30</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1214,16 +1343,19 @@
         <v>5</v>
       </c>
       <c r="C4">
+        <v>502</v>
+      </c>
+      <c r="D4">
         <v>71</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1231,16 +1363,19 @@
         <v>19</v>
       </c>
       <c r="C5">
+        <v>7189</v>
+      </c>
+      <c r="D5">
         <v>385</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1248,16 +1383,19 @@
         <v>26</v>
       </c>
       <c r="C6">
+        <v>16200</v>
+      </c>
+      <c r="D6">
         <v>632</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>59</v>
       </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1265,16 +1403,19 @@
         <v>20</v>
       </c>
       <c r="C7">
+        <v>10088</v>
+      </c>
+      <c r="D7">
         <v>296</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1282,16 +1423,19 @@
         <v>15</v>
       </c>
       <c r="C8">
+        <v>5281</v>
+      </c>
+      <c r="D8">
         <v>60</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1299,12 +1443,15 @@
         <v>7</v>
       </c>
       <c r="C9">
+        <v>522</v>
+      </c>
+      <c r="D9">
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>